<commit_message>
Alteração na escrita das caracteristicas do sinal.
</commit_message>
<xml_diff>
--- a/BasesDeDados/Base1/Codigos_bruno/SegmentacaoManual/FeaturesContracoes.xlsx
+++ b/BasesDeDados/Base1/Codigos_bruno/SegmentacaoManual/FeaturesContracoes.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="618" sheetId="2" r:id="rId2"/>
+    <sheet name="Features" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,12 +26,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Contração</t>
-  </si>
-  <si>
-    <t>RMS</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+  <si>
+    <t>SemanaParto</t>
   </si>
   <si>
     <t>RMS_min</t>
@@ -42,9 +40,6 @@
     <t>RMS_med</t>
   </si>
   <si>
-    <t>VAR</t>
-  </si>
-  <si>
     <t>VAR_min</t>
   </si>
   <si>
@@ -52,6 +47,18 @@
   </si>
   <si>
     <t>VAR_med</t>
+  </si>
+  <si>
+    <t>Dur_med</t>
+  </si>
+  <si>
+    <t>Freq_med</t>
+  </si>
+  <si>
+    <t>Inter_med</t>
+  </si>
+  <si>
+    <t>Arquivo</t>
   </si>
 </sst>
 </file>
@@ -381,15 +388,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,13 +424,98 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>2.542464019705979E-2</v>
+      </c>
+      <c r="C2">
+        <v>4.2254477621555743E-2</v>
+      </c>
+      <c r="D2">
+        <v>3.5883347799831759E-2</v>
+      </c>
+      <c r="E2">
+        <v>1.8374383610610234E-4</v>
+      </c>
+      <c r="F2">
+        <v>8.3908945040467656E-4</v>
+      </c>
+      <c r="G2">
+        <v>5.0625583701139048E-4</v>
+      </c>
+      <c r="H2">
+        <v>60.859090909090916</v>
+      </c>
+      <c r="I2">
+        <v>7.2424407025167472E-3</v>
+      </c>
+      <c r="J2">
+        <v>75.234999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>618</v>
+      </c>
       <c r="B2">
-        <v>3.4188465324821414E-2</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>2.542464019705979E-2</v>
@@ -435,126 +527,22 @@
         <v>3.5883347799831759E-2</v>
       </c>
       <c r="F2">
-        <v>2.9178406724608252E-4</v>
+        <v>1.8374383610610234E-4</v>
       </c>
       <c r="G2">
-        <v>1.8374383610610234E-4</v>
+        <v>8.3908945040467656E-4</v>
       </c>
       <c r="H2">
-        <v>8.3908945040467656E-4</v>
+        <v>5.0625583701139048E-4</v>
       </c>
       <c r="I2">
-        <v>5.0625583701139048E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>3.1685286198763242E-2</v>
-      </c>
-      <c r="F3">
-        <v>2.5136042995518659E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2.542464019705979E-2</v>
-      </c>
-      <c r="F4">
-        <v>1.8374383610610234E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>3.4839937433603425E-2</v>
-      </c>
-      <c r="F5">
-        <v>3.3167146352811608E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>3.030126311014586E-2</v>
-      </c>
-      <c r="F6">
-        <v>6.0729297535085179E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>3.9441977846979767E-2</v>
-      </c>
-      <c r="F7">
-        <v>6.4083991364943121E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>4.2254477621555743E-2</v>
-      </c>
-      <c r="F8">
-        <v>5.9699175616573761E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>3.8585064972579741E-2</v>
-      </c>
-      <c r="F9">
-        <v>5.0646875169312294E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>3.7076355814029398E-2</v>
-      </c>
-      <c r="F10">
-        <v>7.2237484319165139E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>3.9813331926221988E-2</v>
-      </c>
-      <c r="F11">
-        <v>8.3908945040467656E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>4.1106025352389025E-2</v>
-      </c>
-      <c r="F12">
-        <v>5.9719671983433692E-4</v>
+        <v>60.859090909090916</v>
+      </c>
+      <c r="J2">
+        <v>7.2424407025167472E-3</v>
+      </c>
+      <c r="K2">
+        <v>75.234999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Codigo com o filtro de 0.35 a 1  e ONDITAS
</commit_message>
<xml_diff>
--- a/BasesDeDados/Base1/Codigos_bruno/SegmentacaoManual/FeaturesContracoes.xlsx
+++ b/BasesDeDados/Base1/Codigos_bruno/SegmentacaoManual/FeaturesContracoes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\Trabalho1-Fuzzy\BasesDeDados\Base1\Codigos_bruno\SegmentacaoManual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\trabalho1-fuzzy\BasesDeDados\Base1\Codigos_bruno\SegmentacaoManual\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -466,28 +466,28 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>618</v>
+        <v>1022</v>
       </c>
       <c r="B17">
         <v>38</v>
       </c>
       <c r="C17">
-        <v>1.1366622010458653E-2</v>
+        <v>3.3688134922222591E-3</v>
       </c>
       <c r="D17">
-        <v>3.2711627867196266E-2</v>
+        <v>9.5667164284161214E-3</v>
       </c>
       <c r="E17">
-        <v>2.4926750043968646E-2</v>
+        <v>5.1865121585082403E-3</v>
       </c>
       <c r="F17">
-        <v>2.762780974166328E-5</v>
+        <v>1.1102341291114293E-5</v>
       </c>
       <c r="G17">
-        <v>6.0807468370558033E-4</v>
+        <v>4.6030793084526882E-5</v>
       </c>
       <c r="H17">
-        <v>3.2110771534059795E-4</v>
+        <v>2.4555606252025172E-5</v>
       </c>
       <c r="I17">
         <v>101.30000000000001</v>

</xml_diff>

<commit_message>
Mais referencias sobre a entropia arrombada do caralho
</commit_message>
<xml_diff>
--- a/BasesDeDados/Base1/Codigos_bruno/SegmentacaoManual/FeaturesContracoes.xlsx
+++ b/BasesDeDados/Base1/Codigos_bruno/SegmentacaoManual/FeaturesContracoes.xlsx
@@ -466,28 +466,28 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1022</v>
+        <v>618</v>
       </c>
       <c r="B17">
         <v>38</v>
       </c>
       <c r="C17">
-        <v>3.3688134922222591E-3</v>
+        <v>2.6290691919814918E-3</v>
       </c>
       <c r="D17">
-        <v>9.5667164284161214E-3</v>
+        <v>1.8770602169046833E-2</v>
       </c>
       <c r="E17">
-        <v>5.1865121585082403E-3</v>
+        <v>1.3112384595375948E-2</v>
       </c>
       <c r="F17">
-        <v>1.1102341291114293E-5</v>
+        <v>5.5259855144517369E-6</v>
       </c>
       <c r="G17">
-        <v>4.6030793084526882E-5</v>
+        <v>4.2398500789266015E-4</v>
       </c>
       <c r="H17">
-        <v>2.4555606252025172E-5</v>
+        <v>2.284541730856325E-4</v>
       </c>
       <c r="I17">
         <v>101.30000000000001</v>

</xml_diff>